<commit_message>
actually hit save on the spreadsheet
</commit_message>
<xml_diff>
--- a/Search Methods Homework/Search Methods Homework/ExperimentlObservationData.xlsx
+++ b/Search Methods Homework/Search Methods Homework/ExperimentlObservationData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ninja\OneDrive\Documents\School\CS461\Assignment 1\CS461-Program-1-Search-Methods\Search Methods Homework\Search Methods Homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F4E299-5516-453D-97EF-9B4B1E98E24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C582F3-AA70-48CD-9F9A-1F89DFBA5BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>Start</t>
   </si>
@@ -55,6 +55,42 @@
   </si>
   <si>
     <t>Time (Ticks)</t>
+  </si>
+  <si>
+    <t>Hays</t>
+  </si>
+  <si>
+    <t>Topeka</t>
+  </si>
+  <si>
+    <t>Emporia</t>
+  </si>
+  <si>
+    <t>Viola</t>
+  </si>
+  <si>
+    <t>Junction_City</t>
+  </si>
+  <si>
+    <t>Greensburg</t>
+  </si>
+  <si>
+    <t>Augusta</t>
+  </si>
+  <si>
+    <t>Hillsboro</t>
+  </si>
+  <si>
+    <t>Wichita</t>
+  </si>
+  <si>
+    <t>Andover</t>
+  </si>
+  <si>
+    <t>Abilene</t>
+  </si>
+  <si>
+    <t>Leon</t>
   </si>
 </sst>
 </file>
@@ -375,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,6 +518,377 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>217</v>
+      </c>
+      <c r="D3">
+        <v>216</v>
+      </c>
+      <c r="E3">
+        <v>5474</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>4332</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>44</v>
+      </c>
+      <c r="K3">
+        <v>3343</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <v>27</v>
+      </c>
+      <c r="N3">
+        <v>8008</v>
+      </c>
+      <c r="O3">
+        <v>5</v>
+      </c>
+      <c r="P3">
+        <v>5</v>
+      </c>
+      <c r="Q3">
+        <v>109805</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>128</v>
+      </c>
+      <c r="D4">
+        <v>127</v>
+      </c>
+      <c r="E4">
+        <v>5114</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>36</v>
+      </c>
+      <c r="H4">
+        <v>4709</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4">
+        <v>22</v>
+      </c>
+      <c r="K4">
+        <v>2940</v>
+      </c>
+      <c r="L4">
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <v>149</v>
+      </c>
+      <c r="N4">
+        <v>8801</v>
+      </c>
+      <c r="O4">
+        <v>10</v>
+      </c>
+      <c r="P4">
+        <v>14</v>
+      </c>
+      <c r="Q4">
+        <v>107859</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>469</v>
+      </c>
+      <c r="D5">
+        <v>468</v>
+      </c>
+      <c r="E5">
+        <v>781</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>37</v>
+      </c>
+      <c r="H5">
+        <v>811</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>11</v>
+      </c>
+      <c r="K5">
+        <v>434</v>
+      </c>
+      <c r="L5">
+        <v>6</v>
+      </c>
+      <c r="M5">
+        <v>86</v>
+      </c>
+      <c r="N5">
+        <v>828</v>
+      </c>
+      <c r="O5">
+        <v>6</v>
+      </c>
+      <c r="P5">
+        <v>6</v>
+      </c>
+      <c r="Q5">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>261</v>
+      </c>
+      <c r="D6">
+        <v>260</v>
+      </c>
+      <c r="E6">
+        <v>662</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>25</v>
+      </c>
+      <c r="H6">
+        <v>501</v>
+      </c>
+      <c r="I6">
+        <v>14</v>
+      </c>
+      <c r="J6">
+        <v>25</v>
+      </c>
+      <c r="K6">
+        <v>540</v>
+      </c>
+      <c r="L6">
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <v>67</v>
+      </c>
+      <c r="N6">
+        <v>534</v>
+      </c>
+      <c r="O6">
+        <v>6</v>
+      </c>
+      <c r="P6">
+        <v>6</v>
+      </c>
+      <c r="Q6">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>22</v>
+      </c>
+      <c r="D7">
+        <v>21</v>
+      </c>
+      <c r="E7">
+        <v>641</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>17</v>
+      </c>
+      <c r="H7">
+        <v>353</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>182</v>
+      </c>
+      <c r="L7">
+        <v>5</v>
+      </c>
+      <c r="M7">
+        <v>33</v>
+      </c>
+      <c r="N7">
+        <v>500</v>
+      </c>
+      <c r="O7">
+        <v>5</v>
+      </c>
+      <c r="P7">
+        <v>5</v>
+      </c>
+      <c r="Q7">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>29</v>
+      </c>
+      <c r="E8">
+        <v>151</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>187</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>178</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+      <c r="M8">
+        <v>8</v>
+      </c>
+      <c r="N8">
+        <v>1878</v>
+      </c>
+      <c r="O8">
+        <v>6</v>
+      </c>
+      <c r="P8">
+        <v>5</v>
+      </c>
+      <c r="Q8">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>180</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>21</v>
+      </c>
+      <c r="H9">
+        <v>508</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>34</v>
+      </c>
+      <c r="K9">
+        <v>599</v>
+      </c>
+      <c r="L9">
+        <v>8</v>
+      </c>
+      <c r="M9">
+        <v>93</v>
+      </c>
+      <c r="N9">
+        <v>871</v>
+      </c>
+      <c r="O9">
+        <v>8</v>
+      </c>
+      <c r="P9">
+        <v>7</v>
+      </c>
+      <c r="Q9">
+        <v>581</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C1:E1"/>

</xml_diff>